<commit_message>
Added Results of Test Map2/4Ghosts/Level3
</commit_message>
<xml_diff>
--- a/results/Results.xlsx
+++ b/results/Results.xlsx
@@ -5,22 +5,23 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro\Desktop\trabalho-de-grupo-pacman-83808-84681-84715\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5147DF7B-A7ED-45B6-84FB-0194E5ADD93F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E318E73F-6CF0-44AD-A8B5-71AE948F7EA6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13605" xr2:uid="{A44882A2-B556-4762-82F9-DA68A9C0E235}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13605" activeTab="2" xr2:uid="{A44882A2-B556-4762-82F9-DA68A9C0E235}"/>
   </bookViews>
   <sheets>
     <sheet name="Map 2, 2 Ghosts, Level 1" sheetId="3" r:id="rId1"/>
-    <sheet name="Map 2, 4 Ghosts, Level 2" sheetId="1" r:id="rId2"/>
-    <sheet name="Map 2, 4 Ghosts, Level 3" sheetId="5" r:id="rId3"/>
+    <sheet name="Map 2, 4 Ghosts, Level 33" sheetId="5" r:id="rId2"/>
+    <sheet name="Map 2, 4 Ghosts, Level 3" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Map 2, 2 Ghosts, Level 1'!$B$5:$F$37</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Map 2, 4 Ghosts, Level 2'!$B$5:$F$37</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Map 2, 4 Ghosts, Level 3'!$B$5:$F$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Map 2, 4 Ghosts, Level 33'!$B$5:$F$37</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="45">
   <si>
     <t xml:space="preserve"> Ghosts Level 1</t>
   </si>
@@ -77,6 +78,102 @@
   </si>
   <si>
     <t>4 Ghosts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">game_consts__5_4_3.py -&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">game_consts__5_4_4.py -&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">game_consts__5_5_3.py -&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">game_consts__5_5_4.py -&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">game_consts__5_6_3.py -&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">game_consts__5_6_4.py -&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">game_consts__5_7_3.py -&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">game_consts__5_7_4.py -&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">game_consts__6_4_3.py -&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">game_consts__6_4_4.py -&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">game_consts__6_5_3.py -&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">game_consts__6_5_4.py -&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">game_consts__6_6_3.py -&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">game_consts__6_6_4.py -&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">game_consts__6_7_3.py -&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">game_consts__6_7_4.py -&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">game_consts__7_4_3.py -&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">game_consts__7_4_4.py -&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">game_consts__7_5_3.py -&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">game_consts__7_5_4.py -&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">game_consts__7_6_3.py -&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">game_consts__7_6_4.py -&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">game_consts__7_7_3.py -&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">game_consts__7_7_4.py -&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">game_consts__8_4_3.py -&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">game_consts__8_4_4.py -&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">game_consts__8_5_3.py -&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">game_consts__8_5_4.py -&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">game_consts__8_6_3.py -&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">game_consts__8_6_4.py -&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">game_consts__8_7_3.py -&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">game_consts__8_7_4.py -&gt; </t>
   </si>
 </sst>
 </file>
@@ -156,6 +253,2894 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>2 Ghosts Level 1</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Map 2, 2 Ghosts, Level 1'!$F$6:$F$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>894.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>876.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>929.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>931.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>937.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>948.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>950.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>927.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>920.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>941.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>949.4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>926.3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>934.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>937.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>940.8</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>889.1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>925.3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>947.2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>942.6</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>911.6</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>945.3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>971.3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>957.8</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>948.5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>916.4</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>957.2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>924.2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>974.6</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>939.1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>954.5</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>979.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6CDB-4D94-B37E-D628641D1984}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="827805704"/>
+        <c:axId val="827805376"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="827805704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="827805376"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="827805376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="827805704"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>4 Ghosts</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> - </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Level 2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Map 2, 4 Ghosts, Level 33'!$F$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Map 2, 4 Ghosts, Level 33'!$B$6:$B$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Map 2, 4 Ghosts, Level 33'!$F$7:$F$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8710-4676-9BEE-5C6F0846A61F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="798359792"/>
+        <c:axId val="798361432"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="798359792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="798361432"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="798361432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="798359792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>4 Ghosts</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> - </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Level 3</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Map 2, 4 Ghosts, Level 3'!$F$6:$F$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>888.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1017.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>930.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>940.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1070.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>866.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>971.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>881.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>890.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>865.7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1043.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1059.0999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>880.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>557.6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>607.33299999999997</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>841</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1042.4000000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>972.1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>916</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>915.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>986.7</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1060.4000000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1127.5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1023.4</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1004.3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>939.6</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>966.8</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1042</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>881.5</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1025.7</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1015.5</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>952.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E1D3-4312-A215-13F422642F0B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="798359792"/>
+        <c:axId val="798361432"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="798359792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="798361432"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="798361432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="798359792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>50425</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1120</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>313764</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50515FD8-B86B-45C8-8B5F-3069C0CFF0D9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>593912</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>168087</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>554692</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>10085</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{946EBC17-7926-42EA-900F-AC5126C33DC2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>5602</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>34737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>67235</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F6A3896-7B15-423B-827D-C1811954CE12}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0E39F227-939D-4ADC-9C02-19F71105481E}" name="Table13" displayName="Table13" ref="B5:F37" totalsRowShown="0">
   <autoFilter ref="B5:F37" xr:uid="{B2D2ED31-18C7-43D0-9AA8-149FDD648FFB}"/>
@@ -171,6 +3156,20 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A651C61B-8DC1-45DE-A5F2-CABD44C4296B}" name="Table15" displayName="Table15" ref="B5:F37" totalsRowShown="0">
+  <autoFilter ref="B5:F37" xr:uid="{B2D2ED31-18C7-43D0-9AA8-149FDD648FFB}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{E227FE77-79A8-4E15-BF65-3C50D8DFCE95}" name="File #"/>
+    <tableColumn id="2" xr3:uid="{558A4B9D-7B79-4220-AE1E-E3473C039429}" name="SAFE_DIST_TO_GHOST"/>
+    <tableColumn id="3" xr3:uid="{CD07DEAB-17D4-4618-A0D6-219FF7A27B94}" name="GHOST_PURSUIT_MULTIPLIER (*10)"/>
+    <tableColumn id="4" xr3:uid="{DFF817C4-8023-4CC2-A393-5921C9F06FDD}" name="NUMBER_OF_GHOST_TO_OFFENSIVE"/>
+    <tableColumn id="5" xr3:uid="{FFF2181B-C46C-4905-B36E-7C2AAF7102BA}" name="10 Iterations Average"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A33DEB7E-8E24-4154-A688-915E6F908430}" name="Table1" displayName="Table1" ref="B5:F37" totalsRowShown="0">
   <autoFilter ref="B5:F37" xr:uid="{B2D2ED31-18C7-43D0-9AA8-149FDD648FFB}"/>
   <tableColumns count="5">
@@ -179,20 +3178,6 @@
     <tableColumn id="3" xr3:uid="{68D0502A-655A-41B9-A7D4-0E8E17E7CD6D}" name="GHOST_PURSUIT_MULTIPLIER (*10)"/>
     <tableColumn id="4" xr3:uid="{53006559-84DE-4902-9B12-954C6F46CE1F}" name="NUMBER_OF_GHOST_TO_OFFENSIVE"/>
     <tableColumn id="5" xr3:uid="{40C0A9CB-1FAE-4BD4-8712-68EA7BBDDFC1}" name="10 Iterations Average"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A651C61B-8DC1-45DE-A5F2-CABD44C4296B}" name="Table15" displayName="Table15" ref="B5:F37" totalsRowShown="0">
-  <autoFilter ref="B5:F37" xr:uid="{B2D2ED31-18C7-43D0-9AA8-149FDD648FFB}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{E227FE77-79A8-4E15-BF65-3C50D8DFCE95}" name="File #"/>
-    <tableColumn id="2" xr3:uid="{558A4B9D-7B79-4220-AE1E-E3473C039429}" name="SAFE_DIST_TO_GHOST"/>
-    <tableColumn id="3" xr3:uid="{CD07DEAB-17D4-4618-A0D6-219FF7A27B94}" name="GHOST_PURSUIT_MULTIPLIER (*10)"/>
-    <tableColumn id="4" xr3:uid="{DFF817C4-8023-4CC2-A393-5921C9F06FDD}" name="NUMBER_OF_GHOST_TO_OFFENSIVE"/>
-    <tableColumn id="5" xr3:uid="{FFF2181B-C46C-4905-B36E-7C2AAF7102BA}" name="10 Iterations Average"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -497,8 +3482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{433E0203-85C0-4694-979D-4A6D35C9BAE3}">
   <dimension ref="B3:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1100,18 +4085,19 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA26345C-16F1-41D0-B6CF-6E2737431474}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B27BD3D3-2C32-4056-ACEC-12DEEE596D87}">
   <dimension ref="B3:F37"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1128,7 +4114,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>10</v>
@@ -1617,18 +4603,19 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B27BD3D3-2C32-4056-ACEC-12DEEE596D87}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA26345C-16F1-41D0-B6CF-6E2737431474}">
   <dimension ref="B3:F37"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1685,6 +4672,9 @@
       <c r="E6">
         <v>3</v>
       </c>
+      <c r="F6">
+        <v>888.7</v>
+      </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7">
@@ -1699,6 +4689,9 @@
       <c r="E7">
         <v>4</v>
       </c>
+      <c r="F7">
+        <v>1017.4</v>
+      </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8">
@@ -1710,8 +4703,11 @@
       <c r="D8">
         <v>5</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8">
         <v>3</v>
+      </c>
+      <c r="F8">
+        <v>930.6</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -1726,6 +4722,9 @@
       </c>
       <c r="E9">
         <v>4</v>
+      </c>
+      <c r="F9">
+        <v>940.8</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -1741,6 +4740,9 @@
       <c r="E10">
         <v>3</v>
       </c>
+      <c r="F10">
+        <v>1070.3</v>
+      </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11">
@@ -1755,6 +4757,9 @@
       <c r="E11">
         <v>4</v>
       </c>
+      <c r="F11">
+        <v>866.7</v>
+      </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12">
@@ -1769,6 +4774,9 @@
       <c r="E12">
         <v>3</v>
       </c>
+      <c r="F12">
+        <v>971.9</v>
+      </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13">
@@ -1783,6 +4791,9 @@
       <c r="E13">
         <v>4</v>
       </c>
+      <c r="F13">
+        <v>881.2</v>
+      </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14">
@@ -1797,6 +4808,9 @@
       <c r="E14">
         <v>3</v>
       </c>
+      <c r="F14">
+        <v>890.7</v>
+      </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15">
@@ -1811,6 +4825,9 @@
       <c r="E15">
         <v>4</v>
       </c>
+      <c r="F15">
+        <v>865.7</v>
+      </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16">
@@ -1825,8 +4842,11 @@
       <c r="E16">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>1043.7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>12</v>
       </c>
@@ -1839,8 +4859,11 @@
       <c r="E17">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>1059.0999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>13</v>
       </c>
@@ -1853,8 +4876,11 @@
       <c r="E18">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>880.6</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>14</v>
       </c>
@@ -1867,8 +4893,11 @@
       <c r="E19">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>557.6</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>15</v>
       </c>
@@ -1881,8 +4910,11 @@
       <c r="E20">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>607.33299999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>16</v>
       </c>
@@ -1895,8 +4927,11 @@
       <c r="E21">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>17</v>
       </c>
@@ -1909,8 +4944,11 @@
       <c r="E22">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <v>1042.4000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>18</v>
       </c>
@@ -1923,8 +4961,11 @@
       <c r="E23">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <v>972.1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>19</v>
       </c>
@@ -1937,8 +4978,11 @@
       <c r="E24">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>20</v>
       </c>
@@ -1951,8 +4995,11 @@
       <c r="E25">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <v>915.5</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>21</v>
       </c>
@@ -1965,8 +5012,11 @@
       <c r="E26">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <v>986.7</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>22</v>
       </c>
@@ -1979,8 +5029,11 @@
       <c r="E27">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <v>1060.4000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>23</v>
       </c>
@@ -1993,8 +5046,11 @@
       <c r="E28">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <v>1127.5</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>24</v>
       </c>
@@ -2007,8 +5063,11 @@
       <c r="E29">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <v>1023.4</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>25</v>
       </c>
@@ -2021,8 +5080,11 @@
       <c r="E30">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <v>1004.3</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>26</v>
       </c>
@@ -2035,8 +5097,11 @@
       <c r="E31">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <v>939.6</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>27</v>
       </c>
@@ -2049,8 +5114,11 @@
       <c r="E32">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F32">
+        <v>966.8</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>28</v>
       </c>
@@ -2063,8 +5131,11 @@
       <c r="E33">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>29</v>
       </c>
@@ -2077,8 +5148,11 @@
       <c r="E34">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <v>881.5</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>30</v>
       </c>
@@ -2091,8 +5165,11 @@
       <c r="E35">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <v>1025.7</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>31</v>
       </c>
@@ -2105,8 +5182,11 @@
       <c r="E36">
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <v>1015.5</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>32</v>
       </c>
@@ -2118,6 +5198,9 @@
       </c>
       <c r="E37">
         <v>4</v>
+      </c>
+      <c r="F37">
+        <v>952.2</v>
       </c>
     </row>
   </sheetData>
@@ -2134,8 +5217,280 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A54E79CF-581A-4F23-B27F-528D08133068}">
+  <dimension ref="C2:D33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2">
+        <v>888.7</v>
+      </c>
+    </row>
+    <row r="3" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3">
+        <v>1017.4</v>
+      </c>
+    </row>
+    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4">
+        <v>930.6</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5">
+        <v>940.8</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6">
+        <v>1070.3</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7">
+        <v>866.7</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8">
+        <v>971.9</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9">
+        <v>881.2</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10">
+        <v>890.7</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11">
+        <v>865.7</v>
+      </c>
+    </row>
+    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12">
+        <v>1043.7</v>
+      </c>
+    </row>
+    <row r="13" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13">
+        <v>1059.0999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14">
+        <v>880.6</v>
+      </c>
+    </row>
+    <row r="15" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15">
+        <v>557.6</v>
+      </c>
+    </row>
+    <row r="16" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16">
+        <v>607.33299999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18">
+        <v>1042.4000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19">
+        <v>972.1</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21">
+        <v>915.5</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22">
+        <v>986.7</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23">
+        <v>1060.4000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24">
+        <v>1127.5</v>
+      </c>
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25">
+        <v>1023.4</v>
+      </c>
+    </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26">
+        <v>1004.3</v>
+      </c>
+    </row>
+    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27">
+        <v>939.6</v>
+      </c>
+    </row>
+    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28">
+        <v>966.8</v>
+      </c>
+    </row>
+    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30">
+        <v>881.5</v>
+      </c>
+    </row>
+    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31">
+        <v>1025.7</v>
+      </c>
+    </row>
+    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32">
+        <v>1015.5</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>44</v>
+      </c>
+      <c r="D33">
+        <v>952.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>